<commit_message>
Project register updated for first stories
</commit_message>
<xml_diff>
--- a/Docs/Projecto1PR.xlsx
+++ b/Docs/Projecto1PR.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shared folders\Windows\Shared Documents\Collective\Site\Project1\Projecto1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shared folders\Windows\Shared Documents\Collective\Site\Chexman\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413B038B-7B96-4DBA-A18B-C28BC5BA636E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B3DB20-EA09-4CFF-9CD2-A1C478D58FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4350" yWindow="1635" windowWidth="18300" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30195" yWindow="705" windowWidth="18300" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
-    <sheet name="Suggestions" sheetId="2" r:id="rId2"/>
-    <sheet name="Backlog-Epics" sheetId="3" r:id="rId3"/>
-    <sheet name="Backlog-Stories" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
+    <sheet name="Decisions" sheetId="2" r:id="rId2"/>
+    <sheet name="Dod" sheetId="5" r:id="rId3"/>
+    <sheet name="Backlog-Epics" sheetId="3" r:id="rId4"/>
+    <sheet name="Backlog-Stories" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,10 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
-  <si>
-    <t>E002</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="70">
   <si>
     <t>Inception</t>
   </si>
@@ -40,9 +37,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Desciption</t>
-  </si>
-  <si>
     <t>Epic Code</t>
   </si>
   <si>
@@ -67,12 +61,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>I1</t>
-  </si>
-  <si>
-    <t>I1001</t>
-  </si>
-  <si>
     <t>GitHubSet</t>
   </si>
   <si>
@@ -82,9 +70,6 @@
     <t>MLP</t>
   </si>
   <si>
-    <t>I1002</t>
-  </si>
-  <si>
     <t>ReqDoc</t>
   </si>
   <si>
@@ -100,9 +85,6 @@
     <t>EIN</t>
   </si>
   <si>
-    <t>Iº003</t>
-  </si>
-  <si>
     <t>FirstSteps</t>
   </si>
   <si>
@@ -115,9 +97,6 @@
     <t>App name</t>
   </si>
   <si>
-    <t>Suggestion</t>
-  </si>
-  <si>
     <t>proposals</t>
   </si>
   <si>
@@ -128,6 +107,138 @@
   </si>
   <si>
     <t>Provision of basics startup artifacts to define project objectives</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Chexman</t>
+  </si>
+  <si>
+    <t>Tech stack</t>
+  </si>
+  <si>
+    <t>.NET PHP, Java</t>
+  </si>
+  <si>
+    <t>mysql, php,Android</t>
+  </si>
+  <si>
+    <t>Decisions</t>
+  </si>
+  <si>
+    <t>Last Date</t>
+  </si>
+  <si>
+    <t>Deliverables</t>
+  </si>
+  <si>
+    <t>ReqSpec, OverviewMap and Project Register</t>
+  </si>
+  <si>
+    <t>Docs are available to commence work. Additional design odcs to be provided as required.</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>MVP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementation of basic app </t>
+  </si>
+  <si>
+    <t>Not started</t>
+  </si>
+  <si>
+    <t>installable app</t>
+  </si>
+  <si>
+    <t>E1S1</t>
+  </si>
+  <si>
+    <t>E1S2</t>
+  </si>
+  <si>
+    <t>E1S3</t>
+  </si>
+  <si>
+    <t>E2S1</t>
+  </si>
+  <si>
+    <t>MVS Definition</t>
+  </si>
+  <si>
+    <t>Agree and document the MVS</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>E2S2</t>
+  </si>
+  <si>
+    <t>DB Log and User</t>
+  </si>
+  <si>
+    <t>Write the Log and User tables as per Req Spec</t>
+  </si>
+  <si>
+    <t>Assigned</t>
+  </si>
+  <si>
+    <t>Efi</t>
+  </si>
+  <si>
+    <t>E2S3</t>
+  </si>
+  <si>
+    <t>Login Page</t>
+  </si>
+  <si>
+    <t>Write the login page</t>
+  </si>
+  <si>
+    <t>Assigned Jonatan</t>
+  </si>
+  <si>
+    <t>Define first cut style</t>
+  </si>
+  <si>
+    <t>First cut CSS for site</t>
+  </si>
+  <si>
+    <t>E2S4</t>
+  </si>
+  <si>
+    <t>Agree Coding Standards</t>
+  </si>
+  <si>
+    <t>Juanpe to review and all to agree and learn</t>
+  </si>
+  <si>
+    <t>Jonatan</t>
+  </si>
+  <si>
+    <t>Code writen</t>
+  </si>
+  <si>
+    <t>Deliverable uploaded to github</t>
+  </si>
+  <si>
+    <t>Documentation updated as per deliverable</t>
+  </si>
+  <si>
+    <t>performance test</t>
+  </si>
+  <si>
+    <t>Integration test</t>
+  </si>
+  <si>
+    <t>Story updated</t>
   </si>
 </sst>
 </file>
@@ -163,12 +274,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,38 +575,68 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE9047A3-F814-4946-A422-C8267F484FE7}">
-  <dimension ref="B1:E2"/>
+  <dimension ref="B1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="25.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="2">
+        <v>44485</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="2">
+        <v>44492</v>
+      </c>
+      <c r="F3" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -502,43 +646,130 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B760F2-CB8B-4ACA-89C6-D22026A42596}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BADCF265-A119-4463-A610-D7C6C79C636E}">
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B760F2-CB8B-4ACA-89C6-D22026A42596}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="42.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="47.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="3">
+        <v>44496</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="2">
+        <v>44496</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -547,118 +778,195 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F7E5672-F4AF-469B-9F4A-635B0BEE48C0}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="32" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
+        <v>42</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2">
-        <v>44457</v>
+        <v>44492</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
       <c r="F3" s="2">
-        <v>44457</v>
+        <v>44492</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
+        <v>44</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>20</v>
+      </c>
+      <c r="F4" s="2">
+        <v>44492</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BADCF265-A119-4463-A610-D7C6C79C636E}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>